<commit_message>
open files done import window done coal index done base coal done
</commit_message>
<xml_diff>
--- a/原始数据.xlsx
+++ b/原始数据.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="41">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -546,11 +546,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC34"/>
+  <dimension ref="A1:AC38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V2" sqref="V2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F34" sqref="F34:F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -670,73 +670,73 @@
     </row>
     <row r="2" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2">
-        <v>1986</v>
+        <v>1988</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="G2" s="4">
-        <v>27.9</v>
+        <v>28.1</v>
       </c>
       <c r="H2" s="4">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="I2" s="4">
-        <v>70.5</v>
+        <v>75.8</v>
       </c>
       <c r="J2" s="4">
-        <v>0.99596815137211536</v>
+        <v>0.29530974513805286</v>
       </c>
       <c r="K2" s="4">
-        <v>13.8</v>
+        <v>15.6</v>
       </c>
       <c r="L2" s="4">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="M2" s="4">
-        <v>74.599999999999994</v>
+        <v>80.099999999999994</v>
       </c>
       <c r="N2" s="4">
+        <v>6</v>
+      </c>
+      <c r="O2" s="4">
+        <v>2.8</v>
+      </c>
+      <c r="P2" s="4">
+        <v>0.72995314385971188</v>
+      </c>
+      <c r="Q2" s="4">
+        <v>6.7118989874438917</v>
+      </c>
+      <c r="R2" s="4">
         <v>8</v>
       </c>
-      <c r="O2" s="4">
-        <v>2.6</v>
-      </c>
-      <c r="P2" s="4">
-        <v>1.8526336568732862</v>
-      </c>
-      <c r="Q2" s="4">
-        <v>26.231103102440592</v>
-      </c>
-      <c r="R2" s="4">
-        <v>7</v>
-      </c>
       <c r="S2" s="4">
-        <v>1.2</v>
+        <v>0.3</v>
       </c>
       <c r="T2" s="4">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="U2" s="4">
-        <v>2.5999999999999999E-2</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="V2" s="4">
-        <v>1.23</v>
+        <v>2.14</v>
       </c>
       <c r="W2" s="4">
-        <v>1.8989160514346863</v>
+        <v>0.18788849311480899</v>
       </c>
       <c r="X2" s="4" t="s">
         <v>34</v>
@@ -759,73 +759,73 @@
     </row>
     <row r="3" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D3" s="2">
-        <v>1987</v>
+        <v>1993</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="4">
+        <v>28.1</v>
+      </c>
+      <c r="H3" s="4">
+        <v>71</v>
+      </c>
+      <c r="I3" s="4">
+        <v>75.8</v>
+      </c>
+      <c r="J3" s="4">
+        <v>0.29530974513805286</v>
+      </c>
+      <c r="K3" s="4">
+        <v>15.6</v>
+      </c>
+      <c r="L3" s="4">
+        <v>24</v>
+      </c>
+      <c r="M3" s="4">
+        <v>80.099999999999994</v>
+      </c>
+      <c r="N3" s="4">
+        <v>6</v>
+      </c>
+      <c r="O3" s="4">
+        <v>2.8</v>
+      </c>
+      <c r="P3" s="4">
+        <v>0.72995314385971188</v>
+      </c>
+      <c r="Q3" s="4">
+        <v>6.7118989874438917</v>
+      </c>
+      <c r="R3" s="4">
+        <v>8</v>
+      </c>
+      <c r="S3" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="T3" s="4">
         <v>33</v>
       </c>
-      <c r="G3" s="4">
-        <v>29.7</v>
-      </c>
-      <c r="H3" s="4">
-        <v>58</v>
-      </c>
-      <c r="I3" s="4">
-        <v>71.2</v>
-      </c>
-      <c r="J3" s="4">
-        <v>0.78258459905815114</v>
-      </c>
-      <c r="K3" s="4">
-        <v>14.5</v>
-      </c>
-      <c r="L3" s="4">
-        <v>16</v>
-      </c>
-      <c r="M3" s="4">
-        <v>78.599999999999994</v>
-      </c>
-      <c r="N3" s="4">
-        <v>283</v>
-      </c>
-      <c r="O3" s="4">
-        <v>3.1</v>
-      </c>
-      <c r="P3" s="4">
-        <v>3.8137272359694876</v>
-      </c>
-      <c r="Q3" s="4">
-        <v>67.175084911948375</v>
-      </c>
-      <c r="R3" s="4">
-        <v>9</v>
-      </c>
-      <c r="S3" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="T3" s="4">
-        <v>14</v>
-      </c>
       <c r="U3" s="4">
-        <v>3.7999999999999999E-2</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="V3" s="4">
-        <v>1.89</v>
+        <v>2.14</v>
       </c>
       <c r="W3" s="4">
-        <v>4.3903277229662665</v>
+        <v>0.18788849311480899</v>
       </c>
       <c r="X3" s="4" t="s">
         <v>34</v>
@@ -848,7 +848,7 @@
     </row>
     <row r="4" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>29</v>
@@ -857,13 +857,13 @@
         <v>25</v>
       </c>
       <c r="D4" s="2">
-        <v>1988</v>
+        <v>1999</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="G4" s="4">
         <v>28.1</v>
@@ -937,73 +937,73 @@
     </row>
     <row r="5" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" s="2">
-        <v>1989</v>
+        <v>1987</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G5" s="4">
-        <v>26.8</v>
+        <v>29.7</v>
       </c>
       <c r="H5" s="4">
         <v>58</v>
       </c>
       <c r="I5" s="4">
-        <v>85.7</v>
+        <v>71.2</v>
       </c>
       <c r="J5" s="4">
-        <v>0.99094894610458162</v>
+        <v>0.78258459905815114</v>
       </c>
       <c r="K5" s="4">
-        <v>16.899999999999999</v>
+        <v>14.5</v>
       </c>
       <c r="L5" s="4">
-        <v>30.8</v>
+        <v>16</v>
       </c>
       <c r="M5" s="4">
-        <v>73.7</v>
+        <v>78.599999999999994</v>
       </c>
       <c r="N5" s="4">
-        <v>162</v>
+        <v>283</v>
       </c>
       <c r="O5" s="4">
-        <v>2.97</v>
+        <v>3.1</v>
       </c>
       <c r="P5" s="4">
-        <v>4.7461241814077066</v>
+        <v>3.8137272359694876</v>
       </c>
       <c r="Q5" s="4">
-        <v>59.538022734672055</v>
+        <v>67.175084911948375</v>
       </c>
       <c r="R5" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="S5" s="4">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="T5" s="4">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="U5" s="4">
-        <v>5.6000000000000001E-2</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="V5" s="4">
-        <v>2.23</v>
+        <v>1.89</v>
       </c>
       <c r="W5" s="4">
-        <v>2.7820294766421321</v>
+        <v>4.3903277229662665</v>
       </c>
       <c r="X5" s="4" t="s">
         <v>34</v>
@@ -1115,73 +1115,73 @@
     </row>
     <row r="7" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D7" s="2">
-        <v>1991</v>
+        <v>1992</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G7" s="4">
-        <v>27.9</v>
+        <v>29.7</v>
       </c>
       <c r="H7" s="4">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="I7" s="4">
-        <v>70.5</v>
+        <v>71.2</v>
       </c>
       <c r="J7" s="4">
-        <v>0.99596815137211536</v>
+        <v>0.78258459905815114</v>
       </c>
       <c r="K7" s="4">
-        <v>13.8</v>
+        <v>14.5</v>
       </c>
       <c r="L7" s="4">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="M7" s="4">
-        <v>74.599999999999994</v>
+        <v>78.599999999999994</v>
       </c>
       <c r="N7" s="4">
-        <v>8</v>
+        <v>283</v>
       </c>
       <c r="O7" s="4">
-        <v>2.6</v>
+        <v>3.1</v>
       </c>
       <c r="P7" s="4">
-        <v>1.8526336568732862</v>
+        <v>3.8137272359694876</v>
       </c>
       <c r="Q7" s="4">
-        <v>26.231103102440592</v>
+        <v>67.175084911948375</v>
       </c>
       <c r="R7" s="4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="S7" s="4">
-        <v>1.2</v>
+        <v>0.7</v>
       </c>
       <c r="T7" s="4">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="U7" s="4">
-        <v>2.5999999999999999E-2</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="V7" s="4">
-        <v>1.23</v>
+        <v>1.89</v>
       </c>
       <c r="W7" s="4">
-        <v>1.8989160514346863</v>
+        <v>4.3903277229662665</v>
       </c>
       <c r="X7" s="4" t="s">
         <v>34</v>
@@ -1204,7 +1204,7 @@
     </row>
     <row r="8" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>29</v>
@@ -1213,7 +1213,7 @@
         <v>30</v>
       </c>
       <c r="D8" s="2">
-        <v>1992</v>
+        <v>1995</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>26</v>
@@ -1222,55 +1222,55 @@
         <v>37</v>
       </c>
       <c r="G8" s="4">
-        <v>29.7</v>
+        <v>24.3</v>
       </c>
       <c r="H8" s="4">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I8" s="4">
-        <v>71.2</v>
+        <v>72</v>
       </c>
       <c r="J8" s="4">
-        <v>0.78258459905815114</v>
+        <v>0</v>
       </c>
       <c r="K8" s="4">
-        <v>14.5</v>
+        <v>9</v>
       </c>
       <c r="L8" s="4">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="M8" s="4">
-        <v>78.599999999999994</v>
+        <v>70</v>
       </c>
       <c r="N8" s="4">
-        <v>283</v>
+        <v>205</v>
       </c>
       <c r="O8" s="4">
-        <v>3.1</v>
+        <v>1</v>
       </c>
       <c r="P8" s="4">
-        <v>3.8137272359694876</v>
+        <v>2</v>
       </c>
       <c r="Q8" s="4">
-        <v>67.175084911948375</v>
+        <v>59</v>
       </c>
       <c r="R8" s="4">
         <v>9</v>
       </c>
       <c r="S8" s="4">
-        <v>0.7</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="T8" s="4">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="U8" s="4">
-        <v>3.7999999999999999E-2</v>
+        <v>1</v>
       </c>
       <c r="V8" s="4">
-        <v>1.89</v>
+        <v>3</v>
       </c>
       <c r="W8" s="4">
-        <v>4.3903277229662665</v>
+        <v>24</v>
       </c>
       <c r="X8" s="4" t="s">
         <v>34</v>
@@ -1293,73 +1293,73 @@
     </row>
     <row r="9" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D9" s="2">
-        <v>1993</v>
+        <v>1996</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G9" s="4">
-        <v>28.1</v>
+        <v>24.3</v>
       </c>
       <c r="H9" s="4">
-        <v>71</v>
-      </c>
-      <c r="I9" s="4">
-        <v>75.8</v>
-      </c>
-      <c r="J9" s="4">
-        <v>0.29530974513805286</v>
-      </c>
-      <c r="K9" s="4">
-        <v>15.6</v>
-      </c>
-      <c r="L9" s="4">
+        <v>59</v>
+      </c>
+      <c r="I9" s="2">
+        <v>72</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0</v>
+      </c>
+      <c r="K9" s="2">
+        <v>9</v>
+      </c>
+      <c r="L9" s="2">
+        <v>22</v>
+      </c>
+      <c r="M9" s="2">
+        <v>70</v>
+      </c>
+      <c r="N9" s="4">
+        <v>205</v>
+      </c>
+      <c r="O9" s="2">
+        <v>1</v>
+      </c>
+      <c r="P9" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>59</v>
+      </c>
+      <c r="R9" s="4">
+        <v>9</v>
+      </c>
+      <c r="S9" s="4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="T9" s="4">
+        <v>26</v>
+      </c>
+      <c r="U9" s="2">
+        <v>1</v>
+      </c>
+      <c r="V9" s="2">
+        <v>3</v>
+      </c>
+      <c r="W9" s="2">
         <v>24</v>
-      </c>
-      <c r="M9" s="4">
-        <v>80.099999999999994</v>
-      </c>
-      <c r="N9" s="4">
-        <v>6</v>
-      </c>
-      <c r="O9" s="4">
-        <v>2.8</v>
-      </c>
-      <c r="P9" s="4">
-        <v>0.72995314385971188</v>
-      </c>
-      <c r="Q9" s="4">
-        <v>6.7118989874438917</v>
-      </c>
-      <c r="R9" s="4">
-        <v>8</v>
-      </c>
-      <c r="S9" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="T9" s="4">
-        <v>33</v>
-      </c>
-      <c r="U9" s="4">
-        <v>4.1000000000000002E-2</v>
-      </c>
-      <c r="V9" s="4">
-        <v>2.14</v>
-      </c>
-      <c r="W9" s="4">
-        <v>0.18788849311480899</v>
       </c>
       <c r="X9" s="4" t="s">
         <v>34</v>
@@ -1382,73 +1382,73 @@
     </row>
     <row r="10" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" s="2">
-        <v>1994</v>
+        <v>1998</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G10" s="4">
-        <v>26.8</v>
+        <v>29.7</v>
       </c>
       <c r="H10" s="4">
         <v>58</v>
       </c>
       <c r="I10" s="4">
-        <v>85.7</v>
+        <v>71.2</v>
       </c>
       <c r="J10" s="4">
-        <v>0.99094894610458162</v>
+        <v>0.78258459905815114</v>
       </c>
       <c r="K10" s="4">
-        <v>16.899999999999999</v>
+        <v>14.5</v>
       </c>
       <c r="L10" s="4">
-        <v>30.8</v>
+        <v>16</v>
       </c>
       <c r="M10" s="4">
-        <v>73.7</v>
+        <v>78.599999999999994</v>
       </c>
       <c r="N10" s="4">
-        <v>162</v>
+        <v>283</v>
       </c>
       <c r="O10" s="4">
-        <v>2.97</v>
+        <v>3.1</v>
       </c>
       <c r="P10" s="4">
-        <v>4.7461241814077066</v>
+        <v>3.8137272359694876</v>
       </c>
       <c r="Q10" s="4">
-        <v>59.538022734672055</v>
+        <v>67.175084911948375</v>
       </c>
       <c r="R10" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="S10" s="4">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="T10" s="4">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="U10" s="4">
-        <v>5.6000000000000001E-2</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="V10" s="4">
-        <v>2.23</v>
+        <v>1.89</v>
       </c>
       <c r="W10" s="4">
-        <v>2.7820294766421321</v>
+        <v>4.3903277229662665</v>
       </c>
       <c r="X10" s="4" t="s">
         <v>34</v>
@@ -1471,7 +1471,7 @@
     </row>
     <row r="11" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>29</v>
@@ -1480,7 +1480,7 @@
         <v>30</v>
       </c>
       <c r="D11" s="2">
-        <v>1995</v>
+        <v>2001</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>26</v>
@@ -1560,7 +1560,7 @@
     </row>
     <row r="12" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>29</v>
@@ -1569,13 +1569,13 @@
         <v>30</v>
       </c>
       <c r="D12" s="2">
-        <v>1996</v>
+        <v>2002</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G12" s="4">
         <v>24.3</v>
@@ -1583,31 +1583,31 @@
       <c r="H12" s="4">
         <v>59</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="4">
         <v>72</v>
       </c>
-      <c r="J12" s="2">
+      <c r="J12" s="4">
         <v>0</v>
       </c>
-      <c r="K12" s="2">
-        <v>9</v>
-      </c>
-      <c r="L12" s="2">
+      <c r="K12" s="4">
+        <v>9</v>
+      </c>
+      <c r="L12" s="4">
         <v>22</v>
       </c>
-      <c r="M12" s="2">
+      <c r="M12" s="4">
         <v>70</v>
       </c>
       <c r="N12" s="4">
         <v>205</v>
       </c>
-      <c r="O12" s="2">
-        <v>1</v>
-      </c>
-      <c r="P12" s="2">
+      <c r="O12" s="4">
+        <v>1</v>
+      </c>
+      <c r="P12" s="4">
         <v>2</v>
       </c>
-      <c r="Q12" s="2">
+      <c r="Q12" s="4">
         <v>59</v>
       </c>
       <c r="R12" s="4">
@@ -1619,13 +1619,13 @@
       <c r="T12" s="4">
         <v>26</v>
       </c>
-      <c r="U12" s="2">
-        <v>1</v>
-      </c>
-      <c r="V12" s="2">
+      <c r="U12" s="4">
+        <v>1</v>
+      </c>
+      <c r="V12" s="4">
         <v>3</v>
       </c>
-      <c r="W12" s="2">
+      <c r="W12" s="4">
         <v>24</v>
       </c>
       <c r="X12" s="4" t="s">
@@ -1649,73 +1649,73 @@
     </row>
     <row r="13" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D13" s="2">
-        <v>1997</v>
+        <v>2003</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G13" s="4">
-        <v>27.9</v>
+        <v>24.3</v>
       </c>
       <c r="H13" s="4">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="I13" s="4">
-        <v>70.5</v>
+        <v>72</v>
       </c>
       <c r="J13" s="4">
-        <v>0.99596815137211536</v>
+        <v>0</v>
       </c>
       <c r="K13" s="4">
-        <v>13.8</v>
+        <v>9</v>
       </c>
       <c r="L13" s="4">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="M13" s="4">
-        <v>74.599999999999994</v>
+        <v>70</v>
       </c>
       <c r="N13" s="4">
-        <v>8</v>
+        <v>205</v>
       </c>
       <c r="O13" s="4">
-        <v>2.6</v>
+        <v>1</v>
       </c>
       <c r="P13" s="4">
-        <v>1.8526336568732862</v>
+        <v>2</v>
       </c>
       <c r="Q13" s="4">
-        <v>26.231103102440592</v>
+        <v>59</v>
       </c>
       <c r="R13" s="4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="S13" s="4">
-        <v>1.2</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="T13" s="4">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="U13" s="4">
-        <v>2.5999999999999999E-2</v>
+        <v>1</v>
       </c>
       <c r="V13" s="4">
-        <v>1.23</v>
+        <v>3</v>
       </c>
       <c r="W13" s="4">
-        <v>1.8989160514346863</v>
+        <v>24</v>
       </c>
       <c r="X13" s="4" t="s">
         <v>34</v>
@@ -1738,7 +1738,7 @@
     </row>
     <row r="14" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>29</v>
@@ -1747,7 +1747,7 @@
         <v>30</v>
       </c>
       <c r="D14" s="2">
-        <v>1998</v>
+        <v>2004</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>26</v>
@@ -1756,55 +1756,55 @@
         <v>37</v>
       </c>
       <c r="G14" s="4">
-        <v>29.7</v>
+        <v>24.3</v>
       </c>
       <c r="H14" s="4">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I14" s="4">
-        <v>71.2</v>
+        <v>72</v>
       </c>
       <c r="J14" s="4">
-        <v>0.78258459905815114</v>
+        <v>0</v>
       </c>
       <c r="K14" s="4">
-        <v>14.5</v>
+        <v>9</v>
       </c>
       <c r="L14" s="4">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="M14" s="4">
-        <v>78.599999999999994</v>
+        <v>70</v>
       </c>
       <c r="N14" s="4">
-        <v>283</v>
+        <v>205</v>
       </c>
       <c r="O14" s="4">
-        <v>3.1</v>
+        <v>1</v>
       </c>
       <c r="P14" s="4">
-        <v>3.8137272359694876</v>
+        <v>2</v>
       </c>
       <c r="Q14" s="4">
-        <v>67.175084911948375</v>
+        <v>59</v>
       </c>
       <c r="R14" s="4">
         <v>9</v>
       </c>
       <c r="S14" s="4">
-        <v>0.7</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="T14" s="4">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="U14" s="4">
-        <v>3.7999999999999999E-2</v>
+        <v>1</v>
       </c>
       <c r="V14" s="4">
-        <v>1.89</v>
+        <v>3</v>
       </c>
       <c r="W14" s="4">
-        <v>4.3903277229662665</v>
+        <v>24</v>
       </c>
       <c r="X14" s="4" t="s">
         <v>34</v>
@@ -1827,73 +1827,73 @@
     </row>
     <row r="15" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D15" s="2">
-        <v>1999</v>
+        <v>2005</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G15" s="4">
-        <v>28.1</v>
+        <v>24.3</v>
       </c>
       <c r="H15" s="4">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="I15" s="4">
-        <v>75.8</v>
+        <v>72</v>
       </c>
       <c r="J15" s="4">
-        <v>0.29530974513805286</v>
+        <v>0</v>
       </c>
       <c r="K15" s="4">
-        <v>15.6</v>
+        <v>9</v>
       </c>
       <c r="L15" s="4">
+        <v>22</v>
+      </c>
+      <c r="M15" s="4">
+        <v>70</v>
+      </c>
+      <c r="N15" s="4">
+        <v>205</v>
+      </c>
+      <c r="O15" s="4">
+        <v>1</v>
+      </c>
+      <c r="P15" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q15" s="4">
+        <v>59</v>
+      </c>
+      <c r="R15" s="4">
+        <v>9</v>
+      </c>
+      <c r="S15" s="4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="T15" s="4">
+        <v>26</v>
+      </c>
+      <c r="U15" s="4">
+        <v>1</v>
+      </c>
+      <c r="V15" s="4">
+        <v>3</v>
+      </c>
+      <c r="W15" s="4">
         <v>24</v>
-      </c>
-      <c r="M15" s="4">
-        <v>80.099999999999994</v>
-      </c>
-      <c r="N15" s="4">
-        <v>6</v>
-      </c>
-      <c r="O15" s="4">
-        <v>2.8</v>
-      </c>
-      <c r="P15" s="4">
-        <v>0.72995314385971188</v>
-      </c>
-      <c r="Q15" s="4">
-        <v>6.7118989874438917</v>
-      </c>
-      <c r="R15" s="4">
-        <v>8</v>
-      </c>
-      <c r="S15" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="T15" s="4">
-        <v>33</v>
-      </c>
-      <c r="U15" s="4">
-        <v>4.1000000000000002E-2</v>
-      </c>
-      <c r="V15" s="4">
-        <v>2.14</v>
-      </c>
-      <c r="W15" s="4">
-        <v>0.18788849311480899</v>
       </c>
       <c r="X15" s="4" t="s">
         <v>34</v>
@@ -1916,73 +1916,73 @@
     </row>
     <row r="16" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D16" s="2">
-        <v>2000</v>
+        <v>2006</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G16" s="4">
-        <v>26.8</v>
+        <v>24.3</v>
       </c>
       <c r="H16" s="4">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I16" s="4">
-        <v>85.7</v>
+        <v>72</v>
       </c>
       <c r="J16" s="4">
-        <v>0.99094894610458162</v>
+        <v>0</v>
       </c>
       <c r="K16" s="4">
-        <v>16.899999999999999</v>
+        <v>9</v>
       </c>
       <c r="L16" s="4">
-        <v>30.8</v>
+        <v>22</v>
       </c>
       <c r="M16" s="4">
-        <v>73.7</v>
+        <v>70</v>
       </c>
       <c r="N16" s="4">
-        <v>162</v>
+        <v>205</v>
       </c>
       <c r="O16" s="4">
-        <v>2.97</v>
+        <v>1</v>
       </c>
       <c r="P16" s="4">
-        <v>4.7461241814077066</v>
+        <v>2</v>
       </c>
       <c r="Q16" s="4">
-        <v>59.538022734672055</v>
+        <v>59</v>
       </c>
       <c r="R16" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="S16" s="4">
-        <v>0.6</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="T16" s="4">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="U16" s="4">
-        <v>5.6000000000000001E-2</v>
+        <v>1</v>
       </c>
       <c r="V16" s="4">
-        <v>2.23</v>
+        <v>3</v>
       </c>
       <c r="W16" s="4">
-        <v>2.7820294766421321</v>
+        <v>24</v>
       </c>
       <c r="X16" s="4" t="s">
         <v>34</v>
@@ -2005,7 +2005,7 @@
     </row>
     <row r="17" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>29</v>
@@ -2014,7 +2014,7 @@
         <v>30</v>
       </c>
       <c r="D17" s="2">
-        <v>2001</v>
+        <v>2007</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>26</v>
@@ -2094,7 +2094,7 @@
     </row>
     <row r="18" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>29</v>
@@ -2103,7 +2103,7 @@
         <v>30</v>
       </c>
       <c r="D18" s="2">
-        <v>2002</v>
+        <v>2008</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>26</v>
@@ -2183,7 +2183,7 @@
     </row>
     <row r="19" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>29</v>
@@ -2192,7 +2192,7 @@
         <v>30</v>
       </c>
       <c r="D19" s="2">
-        <v>2003</v>
+        <v>2009</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>26</v>
@@ -2272,7 +2272,7 @@
     </row>
     <row r="20" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>29</v>
@@ -2281,7 +2281,7 @@
         <v>30</v>
       </c>
       <c r="D20" s="2">
-        <v>2004</v>
+        <v>2010</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>26</v>
@@ -2361,7 +2361,7 @@
     </row>
     <row r="21" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>29</v>
@@ -2370,7 +2370,7 @@
         <v>30</v>
       </c>
       <c r="D21" s="2">
-        <v>2005</v>
+        <v>2011</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>26</v>
@@ -2450,7 +2450,7 @@
     </row>
     <row r="22" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>29</v>
@@ -2459,7 +2459,7 @@
         <v>30</v>
       </c>
       <c r="D22" s="2">
-        <v>2006</v>
+        <v>2012</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>26</v>
@@ -2539,7 +2539,7 @@
     </row>
     <row r="23" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>29</v>
@@ -2548,7 +2548,7 @@
         <v>30</v>
       </c>
       <c r="D23" s="2">
-        <v>2007</v>
+        <v>2013</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>26</v>
@@ -2628,7 +2628,7 @@
     </row>
     <row r="24" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>29</v>
@@ -2637,7 +2637,7 @@
         <v>30</v>
       </c>
       <c r="D24" s="2">
-        <v>2008</v>
+        <v>2014</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>26</v>
@@ -2717,7 +2717,7 @@
     </row>
     <row r="25" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>29</v>
@@ -2726,7 +2726,7 @@
         <v>30</v>
       </c>
       <c r="D25" s="2">
-        <v>2009</v>
+        <v>2015</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>26</v>
@@ -2806,7 +2806,7 @@
     </row>
     <row r="26" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>29</v>
@@ -2815,7 +2815,7 @@
         <v>30</v>
       </c>
       <c r="D26" s="2">
-        <v>2010</v>
+        <v>2016</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>26</v>
@@ -2895,7 +2895,7 @@
     </row>
     <row r="27" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>29</v>
@@ -2904,7 +2904,7 @@
         <v>30</v>
       </c>
       <c r="D27" s="2">
-        <v>2011</v>
+        <v>2017</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>26</v>
@@ -2984,7 +2984,7 @@
     </row>
     <row r="28" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>29</v>
@@ -2993,7 +2993,7 @@
         <v>30</v>
       </c>
       <c r="D28" s="2">
-        <v>2012</v>
+        <v>2018</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>26</v>
@@ -3073,73 +3073,73 @@
     </row>
     <row r="29" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D29" s="2">
-        <v>2013</v>
+        <v>1986</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G29" s="4">
-        <v>24.3</v>
+        <v>27.9</v>
       </c>
       <c r="H29" s="4">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="I29" s="4">
-        <v>72</v>
+        <v>70.5</v>
       </c>
       <c r="J29" s="4">
-        <v>0</v>
+        <v>0.99596815137211536</v>
       </c>
       <c r="K29" s="4">
-        <v>9</v>
+        <v>13.8</v>
       </c>
       <c r="L29" s="4">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="M29" s="4">
-        <v>70</v>
+        <v>74.599999999999994</v>
       </c>
       <c r="N29" s="4">
-        <v>205</v>
+        <v>8</v>
       </c>
       <c r="O29" s="4">
-        <v>1</v>
+        <v>2.6</v>
       </c>
       <c r="P29" s="4">
-        <v>2</v>
+        <v>1.8526336568732862</v>
       </c>
       <c r="Q29" s="4">
-        <v>59</v>
+        <v>26.231103102440592</v>
       </c>
       <c r="R29" s="4">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="S29" s="4">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
       <c r="T29" s="4">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="U29" s="4">
-        <v>1</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="V29" s="4">
-        <v>3</v>
+        <v>1.23</v>
       </c>
       <c r="W29" s="4">
-        <v>24</v>
+        <v>1.8989160514346863</v>
       </c>
       <c r="X29" s="4" t="s">
         <v>34</v>
@@ -3162,73 +3162,73 @@
     </row>
     <row r="30" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D30" s="2">
-        <v>2014</v>
+        <v>1989</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G30" s="4">
-        <v>24.3</v>
+        <v>26.8</v>
       </c>
       <c r="H30" s="4">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I30" s="4">
-        <v>72</v>
+        <v>85.7</v>
       </c>
       <c r="J30" s="4">
-        <v>0</v>
+        <v>0.99094894610458162</v>
       </c>
       <c r="K30" s="4">
-        <v>9</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="L30" s="4">
-        <v>22</v>
+        <v>30.8</v>
       </c>
       <c r="M30" s="4">
-        <v>70</v>
+        <v>73.7</v>
       </c>
       <c r="N30" s="4">
-        <v>205</v>
+        <v>162</v>
       </c>
       <c r="O30" s="4">
-        <v>1</v>
+        <v>2.97</v>
       </c>
       <c r="P30" s="4">
-        <v>2</v>
+        <v>4.7461241814077066</v>
       </c>
       <c r="Q30" s="4">
-        <v>59</v>
+        <v>59.538022734672055</v>
       </c>
       <c r="R30" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S30" s="4">
-        <v>1.1000000000000001</v>
+        <v>0.6</v>
       </c>
       <c r="T30" s="4">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="U30" s="4">
-        <v>1</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="V30" s="4">
-        <v>3</v>
+        <v>2.23</v>
       </c>
       <c r="W30" s="4">
-        <v>24</v>
+        <v>2.7820294766421321</v>
       </c>
       <c r="X30" s="4" t="s">
         <v>34</v>
@@ -3251,73 +3251,73 @@
     </row>
     <row r="31" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D31" s="2">
-        <v>2015</v>
+        <v>1991</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G31" s="4">
-        <v>24.3</v>
+        <v>27.9</v>
       </c>
       <c r="H31" s="4">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="I31" s="4">
-        <v>72</v>
+        <v>70.5</v>
       </c>
       <c r="J31" s="4">
-        <v>0</v>
+        <v>0.99596815137211536</v>
       </c>
       <c r="K31" s="4">
-        <v>9</v>
+        <v>13.8</v>
       </c>
       <c r="L31" s="4">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="M31" s="4">
-        <v>70</v>
+        <v>74.599999999999994</v>
       </c>
       <c r="N31" s="4">
-        <v>205</v>
+        <v>8</v>
       </c>
       <c r="O31" s="4">
-        <v>1</v>
+        <v>2.6</v>
       </c>
       <c r="P31" s="4">
-        <v>2</v>
+        <v>1.8526336568732862</v>
       </c>
       <c r="Q31" s="4">
-        <v>59</v>
+        <v>26.231103102440592</v>
       </c>
       <c r="R31" s="4">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="S31" s="4">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
       <c r="T31" s="4">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="U31" s="4">
-        <v>1</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="V31" s="4">
-        <v>3</v>
+        <v>1.23</v>
       </c>
       <c r="W31" s="4">
-        <v>24</v>
+        <v>1.8989160514346863</v>
       </c>
       <c r="X31" s="4" t="s">
         <v>34</v>
@@ -3340,73 +3340,73 @@
     </row>
     <row r="32" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D32" s="2">
-        <v>2016</v>
+        <v>1994</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G32" s="4">
-        <v>24.3</v>
+        <v>26.8</v>
       </c>
       <c r="H32" s="4">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I32" s="4">
-        <v>72</v>
+        <v>85.7</v>
       </c>
       <c r="J32" s="4">
-        <v>0</v>
+        <v>0.99094894610458162</v>
       </c>
       <c r="K32" s="4">
-        <v>9</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="L32" s="4">
-        <v>22</v>
+        <v>30.8</v>
       </c>
       <c r="M32" s="4">
-        <v>70</v>
+        <v>73.7</v>
       </c>
       <c r="N32" s="4">
-        <v>205</v>
+        <v>162</v>
       </c>
       <c r="O32" s="4">
-        <v>1</v>
+        <v>2.97</v>
       </c>
       <c r="P32" s="4">
-        <v>2</v>
+        <v>4.7461241814077066</v>
       </c>
       <c r="Q32" s="4">
-        <v>59</v>
+        <v>59.538022734672055</v>
       </c>
       <c r="R32" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S32" s="4">
-        <v>1.1000000000000001</v>
+        <v>0.6</v>
       </c>
       <c r="T32" s="4">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="U32" s="4">
-        <v>1</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="V32" s="4">
-        <v>3</v>
+        <v>2.23</v>
       </c>
       <c r="W32" s="4">
-        <v>24</v>
+        <v>2.7820294766421321</v>
       </c>
       <c r="X32" s="4" t="s">
         <v>34</v>
@@ -3429,73 +3429,73 @@
     </row>
     <row r="33" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D33" s="2">
-        <v>2017</v>
+        <v>1997</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G33" s="4">
-        <v>24.3</v>
+        <v>27.9</v>
       </c>
       <c r="H33" s="4">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="I33" s="4">
-        <v>72</v>
+        <v>70.5</v>
       </c>
       <c r="J33" s="4">
-        <v>0</v>
+        <v>0.99596815137211536</v>
       </c>
       <c r="K33" s="4">
-        <v>9</v>
+        <v>13.8</v>
       </c>
       <c r="L33" s="4">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="M33" s="4">
-        <v>70</v>
+        <v>74.599999999999994</v>
       </c>
       <c r="N33" s="4">
-        <v>205</v>
+        <v>8</v>
       </c>
       <c r="O33" s="4">
-        <v>1</v>
+        <v>2.6</v>
       </c>
       <c r="P33" s="4">
-        <v>2</v>
+        <v>1.8526336568732862</v>
       </c>
       <c r="Q33" s="4">
-        <v>59</v>
+        <v>26.231103102440592</v>
       </c>
       <c r="R33" s="4">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="S33" s="4">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
       <c r="T33" s="4">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="U33" s="4">
-        <v>1</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="V33" s="4">
-        <v>3</v>
+        <v>1.23</v>
       </c>
       <c r="W33" s="4">
-        <v>24</v>
+        <v>1.8989160514346863</v>
       </c>
       <c r="X33" s="4" t="s">
         <v>34</v>
@@ -3518,94 +3518,453 @@
     </row>
     <row r="34" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C34" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D34" s="2">
+        <v>2000</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G34" s="4">
+        <v>26.8</v>
+      </c>
+      <c r="H34" s="4">
+        <v>58</v>
+      </c>
+      <c r="I34" s="4">
+        <v>85.7</v>
+      </c>
+      <c r="J34" s="4">
+        <v>0.99094894610458162</v>
+      </c>
+      <c r="K34" s="4">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="L34" s="4">
+        <v>30.8</v>
+      </c>
+      <c r="M34" s="4">
+        <v>73.7</v>
+      </c>
+      <c r="N34" s="4">
+        <v>162</v>
+      </c>
+      <c r="O34" s="4">
+        <v>2.97</v>
+      </c>
+      <c r="P34" s="4">
+        <v>4.7461241814077066</v>
+      </c>
+      <c r="Q34" s="4">
+        <v>59.538022734672055</v>
+      </c>
+      <c r="R34" s="4">
+        <v>8</v>
+      </c>
+      <c r="S34" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="T34" s="4">
+        <v>16</v>
+      </c>
+      <c r="U34" s="4">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="V34" s="4">
+        <v>2.23</v>
+      </c>
+      <c r="W34" s="4">
+        <v>2.7820294766421321</v>
+      </c>
+      <c r="X34" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y34" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z34" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA34" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB34" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC34" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="2">
         <v>30</v>
       </c>
-      <c r="D34" s="2">
+      <c r="B35" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D35" s="2">
+        <v>2015</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G35" s="4">
+        <v>24.3</v>
+      </c>
+      <c r="H35" s="4">
+        <v>59</v>
+      </c>
+      <c r="I35" s="4">
+        <v>72</v>
+      </c>
+      <c r="J35" s="4">
+        <v>0</v>
+      </c>
+      <c r="K35" s="4">
+        <v>9</v>
+      </c>
+      <c r="L35" s="4">
+        <v>22</v>
+      </c>
+      <c r="M35" s="4">
+        <v>70</v>
+      </c>
+      <c r="N35" s="4">
+        <v>205</v>
+      </c>
+      <c r="O35" s="4">
+        <v>1</v>
+      </c>
+      <c r="P35" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q35" s="4">
+        <v>59</v>
+      </c>
+      <c r="R35" s="4">
+        <v>9</v>
+      </c>
+      <c r="S35" s="4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="T35" s="4">
+        <v>26</v>
+      </c>
+      <c r="U35" s="4">
+        <v>1</v>
+      </c>
+      <c r="V35" s="4">
+        <v>3</v>
+      </c>
+      <c r="W35" s="4">
+        <v>24</v>
+      </c>
+      <c r="X35" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y35" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z35" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA35" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB35" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC35" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="2">
+        <v>31</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D36" s="2">
+        <v>2016</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G36" s="4">
+        <v>24.3</v>
+      </c>
+      <c r="H36" s="4">
+        <v>59</v>
+      </c>
+      <c r="I36" s="4">
+        <v>72</v>
+      </c>
+      <c r="J36" s="4">
+        <v>0</v>
+      </c>
+      <c r="K36" s="4">
+        <v>9</v>
+      </c>
+      <c r="L36" s="4">
+        <v>22</v>
+      </c>
+      <c r="M36" s="4">
+        <v>70</v>
+      </c>
+      <c r="N36" s="4">
+        <v>205</v>
+      </c>
+      <c r="O36" s="4">
+        <v>1</v>
+      </c>
+      <c r="P36" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q36" s="4">
+        <v>59</v>
+      </c>
+      <c r="R36" s="4">
+        <v>9</v>
+      </c>
+      <c r="S36" s="4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="T36" s="4">
+        <v>26</v>
+      </c>
+      <c r="U36" s="4">
+        <v>1</v>
+      </c>
+      <c r="V36" s="4">
+        <v>3</v>
+      </c>
+      <c r="W36" s="4">
+        <v>24</v>
+      </c>
+      <c r="X36" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y36" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z36" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA36" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB36" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC36" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="2">
+        <v>32</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D37" s="2">
+        <v>2017</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G37" s="4">
+        <v>24.3</v>
+      </c>
+      <c r="H37" s="4">
+        <v>59</v>
+      </c>
+      <c r="I37" s="4">
+        <v>72</v>
+      </c>
+      <c r="J37" s="4">
+        <v>0</v>
+      </c>
+      <c r="K37" s="4">
+        <v>9</v>
+      </c>
+      <c r="L37" s="4">
+        <v>22</v>
+      </c>
+      <c r="M37" s="4">
+        <v>70</v>
+      </c>
+      <c r="N37" s="4">
+        <v>205</v>
+      </c>
+      <c r="O37" s="4">
+        <v>1</v>
+      </c>
+      <c r="P37" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q37" s="4">
+        <v>59</v>
+      </c>
+      <c r="R37" s="4">
+        <v>9</v>
+      </c>
+      <c r="S37" s="4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="T37" s="4">
+        <v>26</v>
+      </c>
+      <c r="U37" s="4">
+        <v>1</v>
+      </c>
+      <c r="V37" s="4">
+        <v>3</v>
+      </c>
+      <c r="W37" s="4">
+        <v>24</v>
+      </c>
+      <c r="X37" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y37" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z37" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA37" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB37" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC37" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="2">
+        <v>33</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D38" s="2">
         <v>2018</v>
       </c>
-      <c r="E34" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G34" s="4">
+      <c r="E38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G38" s="4">
         <v>24.3</v>
       </c>
-      <c r="H34" s="4">
-        <v>59</v>
-      </c>
-      <c r="I34" s="4">
+      <c r="H38" s="4">
+        <v>59</v>
+      </c>
+      <c r="I38" s="4">
         <v>72</v>
       </c>
-      <c r="J34" s="4">
+      <c r="J38" s="4">
         <v>0</v>
       </c>
-      <c r="K34" s="4">
-        <v>9</v>
-      </c>
-      <c r="L34" s="4">
+      <c r="K38" s="4">
+        <v>9</v>
+      </c>
+      <c r="L38" s="4">
         <v>22</v>
       </c>
-      <c r="M34" s="4">
+      <c r="M38" s="4">
         <v>70</v>
       </c>
-      <c r="N34" s="4">
+      <c r="N38" s="4">
         <v>205</v>
       </c>
-      <c r="O34" s="4">
-        <v>1</v>
-      </c>
-      <c r="P34" s="4">
+      <c r="O38" s="4">
+        <v>1</v>
+      </c>
+      <c r="P38" s="4">
         <v>2</v>
       </c>
-      <c r="Q34" s="4">
-        <v>59</v>
-      </c>
-      <c r="R34" s="4">
-        <v>9</v>
-      </c>
-      <c r="S34" s="4">
+      <c r="Q38" s="4">
+        <v>59</v>
+      </c>
+      <c r="R38" s="4">
+        <v>9</v>
+      </c>
+      <c r="S38" s="4">
         <v>1.1000000000000001</v>
       </c>
-      <c r="T34" s="4">
-        <v>26</v>
-      </c>
-      <c r="U34" s="4">
-        <v>1</v>
-      </c>
-      <c r="V34" s="4">
+      <c r="T38" s="4">
+        <v>26</v>
+      </c>
+      <c r="U38" s="4">
+        <v>1</v>
+      </c>
+      <c r="V38" s="4">
         <v>3</v>
       </c>
-      <c r="W34" s="4">
+      <c r="W38" s="4">
         <v>24</v>
       </c>
-      <c r="X34" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y34" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z34" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA34" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="AB34" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="AC34" s="4" t="s">
+      <c r="X38" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y38" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z38" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA38" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB38" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC38" s="4" t="s">
         <v>34</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:AC34">
+    <sortCondition ref="C2:C34"/>
+  </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>